<commit_message>
number of jobs vs 1 node time done
</commit_message>
<xml_diff>
--- a/genome_data/processed_data/differentjobs-1node-30k.xlsx
+++ b/genome_data/processed_data/differentjobs-1node-30k.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwarade/Desktop/phd-support/genome_data/processed_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\phd-support\genome_data\processed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEE2F1A-8785-2D41-B8CA-8496152736DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9455854-31A2-4A84-8B29-76CB26234DBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -34,22 +34,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>job number</t>
   </si>
   <si>
     <t>1node time</t>
   </si>
+  <si>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>30k</t>
+  </si>
+  <si>
+    <t>energy consumption</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -75,8 +90,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -97,7 +116,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -184,20 +203,47 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>overview!$B$14:$B$17</c:f>
+              <c:f>overview!$B$14:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="10">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="12">
                   <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
@@ -205,20 +251,32 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>overview!$C$14:$C$17</c:f>
+              <c:f>overview!$C$14:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
+                  <c:v>40595</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21873</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15609</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>19721</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>15855</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="10">
                   <c:v>17229</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
                   <c:v>19013</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="12">
                   <c:v>21455</c:v>
                 </c:pt>
               </c:numCache>
@@ -227,7 +285,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D2E6-4617-92B6-3382CA1D4A96}"/>
+              <c16:uniqueId val="{00000000-07C2-45FC-BDE5-9FFD33129975}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -239,13 +297,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="831584320"/>
-        <c:axId val="831579328"/>
+        <c:axId val="1901936848"/>
+        <c:axId val="104235648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="831584320"/>
+        <c:axId val="1901936848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="11"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -270,7 +329,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-AU"/>
-                  <a:t>Number of individual jobs</a:t>
+                  <a:t>Number of jobs</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -341,16 +400,15 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="831579328"/>
+        <c:crossAx val="104235648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="5"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="831579328"/>
+        <c:axId val="104235648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="12000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -389,8 +447,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-AU"/>
-                  <a:t>Time</a:t>
+                  <a:t>Execution</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -460,7 +523,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="831584320"/>
+        <c:crossAx val="1901936848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1100,23 +1163,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{037525F7-F452-4F88-8DD0-FCB6717AD87A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA01A6ED-4997-4281-800E-14FB380A8190}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1400,52 +1463,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B13:C17"/>
+  <dimension ref="B12:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="AB26" sqref="AB26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>40595</v>
+      </c>
+      <c r="D14" s="1">
+        <v>4.3953371820999996</v>
+      </c>
+      <c r="E14">
+        <f>D14*C14/3600</f>
+        <v>49.563531363152634</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1">
+        <v>21873</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5.2587864612999997</v>
+      </c>
+      <c r="E15">
+        <f>D15*C15/3600</f>
+        <v>31.951510074448581</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1">
+        <v>15609</v>
+      </c>
+      <c r="D16" s="2">
+        <v>6.0091125071774902</v>
+      </c>
+      <c r="E16">
+        <f>D16*C16/3600</f>
+        <v>26.054510312370404</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>D17*C17/3600</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>5</v>
+      </c>
+      <c r="C18" s="1">
+        <v>19721</v>
+      </c>
+      <c r="D18" s="2">
+        <v>5.4825246515473403</v>
+      </c>
+      <c r="E18">
+        <f>D18*C18/3600</f>
+        <v>30.033574625879197</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>6</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f>D19*C19/3600</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <f>D20*C20/3600</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <f>D21*C21/3600</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>9</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <f>D22*C22/3600</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
         <v>10</v>
       </c>
-      <c r="C14">
+      <c r="C23" s="1">
         <v>15855</v>
       </c>
+      <c r="D23" s="1">
+        <v>6.0575252531905299</v>
+      </c>
+      <c r="E23">
+        <f>D23*C23/3600</f>
+        <v>26.678350802593293</v>
+      </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
         <v>25</v>
       </c>
-      <c r="C15">
+      <c r="C24" s="1">
         <v>17229</v>
       </c>
+      <c r="D24" s="1">
+        <v>5.9651309764482798</v>
+      </c>
+      <c r="E24">
+        <f>D24*C24/3600</f>
+        <v>28.548122664785392</v>
+      </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B16">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
         <v>50</v>
       </c>
-      <c r="C16">
+      <c r="C25" s="1">
         <v>19013</v>
       </c>
+      <c r="D25" s="1">
+        <v>5.6800410353510999</v>
+      </c>
+      <c r="E25">
+        <f>D25*C25/3600</f>
+        <v>29.998505612536238</v>
+      </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B17">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
         <v>75</v>
       </c>
-      <c r="C17">
+      <c r="C26" s="1">
         <v>21455</v>
+      </c>
+      <c r="D26" s="1">
+        <v>5.3997713678906702</v>
+      </c>
+      <c r="E26">
+        <f>D26*C26/3600</f>
+        <v>32.181137416137311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
different number of jobs 30k done
</commit_message>
<xml_diff>
--- a/genome_data/processed_data/differentjobs-1node-30k.xlsx
+++ b/genome_data/processed_data/differentjobs-1node-30k.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\phd-support\genome_data\processed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A228669-55F0-4601-A4B6-6DFB96473709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398FFFFF-5092-4985-9569-947EA9C02611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,10 +203,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>overview!$B$14:$B$26</c:f>
+              <c:f>overview!$B$14:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -236,25 +236,16 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>overview!$C$14:$C$26</c:f>
+              <c:f>overview!$C$14:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>40595</c:v>
                 </c:pt>
@@ -264,23 +255,26 @@
                 <c:pt idx="2">
                   <c:v>15609</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>12821</c:v>
+                </c:pt>
                 <c:pt idx="4">
                   <c:v>19721</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>17746</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>15440</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15462</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19020</c:v>
+                </c:pt>
                 <c:pt idx="9">
                   <c:v>15855</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>17229</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>19013</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>21455</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -332,7 +326,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-AU"/>
-                  <a:t>Number of jobs</a:t>
+                  <a:t>Number of individual jobs</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1166,16 +1160,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>180974</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>390524</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>342899</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>552449</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1469,7 +1463,7 @@
   <dimension ref="B12:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I17" activeCellId="1" sqref="I32 I17"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,12 +1539,15 @@
       <c r="B17" s="1">
         <v>4</v>
       </c>
+      <c r="C17" s="1">
+        <v>12821</v>
+      </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>6.4207000000000001</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22.866609638888889</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -1587,36 +1584,45 @@
       <c r="B20" s="1">
         <v>7</v>
       </c>
+      <c r="C20" s="1">
+        <v>15440</v>
+      </c>
       <c r="D20" s="1">
-        <v>0</v>
+        <v>6.0654479520000004</v>
       </c>
       <c r="E20" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26.014032327466669</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>8</v>
       </c>
+      <c r="C21" s="1">
+        <v>15462</v>
+      </c>
       <c r="D21" s="1">
-        <v>0</v>
+        <v>6.0418915999999996</v>
       </c>
       <c r="E21" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25.949924421999999</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>9</v>
       </c>
+      <c r="C22" s="1">
+        <v>19020</v>
+      </c>
       <c r="D22" s="1">
-        <v>0</v>
+        <v>5.5562459999999998</v>
       </c>
       <c r="E22" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>29.355499699999999</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
edits for jean-guy. folder change and extract data change
</commit_message>
<xml_diff>
--- a/genome_data/processed_data/differentjobs-1node-30k.xlsx
+++ b/genome_data/processed_data/differentjobs-1node-30k.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\phd-support\genome_data\processed_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwarade/Desktop/phd-support/genome_data/processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398FFFFF-5092-4985-9569-947EA9C02611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F90173-095C-2549-97D1-96C368F90B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>job number</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>energy consumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -116,7 +119,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -127,36 +130,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -296,6 +269,135 @@
         </c:dLbls>
         <c:axId val="1901936848"/>
         <c:axId val="104235648"/>
+      </c:scatterChart>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>energy</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>overview!$B$14:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>overview!$E$14:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>49.563531363152634</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31.951510074448581</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.054510312370404</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22.866609638888889</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30.033574625879197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.02370267628401</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.014032327466669</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25.949924421999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.355499699999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26.678350802593293</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6D0D-2644-95B0-180E9889F505}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2139151983"/>
+        <c:axId val="2049690159"/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="1901936848"/>
@@ -524,6 +626,68 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+      <c:valAx>
+        <c:axId val="2049690159"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2139151983"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2139151983"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2049690159"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1460,23 +1624,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B12:E26"/>
+  <dimension ref="B12:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C12" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1490,7 +1654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>1</v>
       </c>
@@ -1505,7 +1669,7 @@
         <v>49.563531363152634</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>2</v>
       </c>
@@ -1520,7 +1684,7 @@
         <v>31.951510074448581</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>3</v>
       </c>
@@ -1535,7 +1699,7 @@
         <v>26.054510312370404</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
         <v>4</v>
       </c>
@@ -1550,7 +1714,7 @@
         <v>22.866609638888889</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
         <v>5</v>
       </c>
@@ -1565,7 +1729,7 @@
         <v>30.033574625879197</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>6</v>
       </c>
@@ -1580,7 +1744,7 @@
         <v>28.02370267628401</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
         <v>7</v>
       </c>
@@ -1595,7 +1759,7 @@
         <v>26.014032327466669</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>8</v>
       </c>
@@ -1610,7 +1774,7 @@
         <v>25.949924421999999</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="1">
         <v>9</v>
       </c>
@@ -1625,7 +1789,7 @@
         <v>29.355499699999999</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="1">
         <v>10</v>
       </c>
@@ -1640,7 +1804,7 @@
         <v>26.678350802593293</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
         <v>25</v>
       </c>
@@ -1655,7 +1819,7 @@
         <v>28.548122664785392</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
         <v>50</v>
       </c>
@@ -1670,7 +1834,7 @@
         <v>29.998505612536238</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
         <v>75</v>
       </c>
@@ -1683,6 +1847,11 @@
       <c r="E26" s="1">
         <f t="shared" si="0"/>
         <v>32.181137416137311</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G33" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
folder and file structure changed
</commit_message>
<xml_diff>
--- a/genome_data/processed_data/differentjobs-1node-30k.xlsx
+++ b/genome_data/processed_data/differentjobs-1node-30k.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mwarade/Desktop/phd-support/genome_data/processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F90173-095C-2549-97D1-96C368F90B0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25F7441-AC01-AE48-B1AF-20042D201E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -276,9 +276,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>energy</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -686,6 +683,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="2049690159"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1627,7 +1625,7 @@
   <dimension ref="B12:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>